<commit_message>
Monthly Feed and Prices
</commit_message>
<xml_diff>
--- a/spread.xlsx
+++ b/spread.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t xml:space="preserve">Misc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feed per Pig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feed per Pig per age</t>
   </si>
 </sst>
 </file>
@@ -206,7 +215,7 @@
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="12.94"/>
@@ -447,15 +456,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.74"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="n">
+        <v>2021</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -535,15 +550,139 @@
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>644</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>